<commit_message>
Added new item icons.
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\production-line\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4B01B4-BF26-4333-A489-420FB9E97442}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDDAF0A6-DDB6-4094-B1D1-37FD70717ED2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="37110" windowHeight="14625" xr2:uid="{90F13507-3F9A-4BE5-82EE-4FDD9857C5A2}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Guide to Uses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="181">
   <si>
     <t>Item</t>
   </si>
@@ -505,9 +506,6 @@
     <t>13 Nails</t>
   </si>
   <si>
-    <t>13 Nails: 1</t>
-  </si>
-  <si>
     <t>Battery</t>
   </si>
   <si>
@@ -575,6 +573,9 @@
   </si>
   <si>
     <t>Chip: 1, Zinc Coil: 1</t>
+  </si>
+  <si>
+    <t>13 Nails: 1, Coal: 1</t>
   </si>
 </sst>
 </file>
@@ -656,21 +657,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -997,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642C1486-BA39-4873-8BE1-FD047E7D1A0C}">
   <dimension ref="A1:I80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1019,7 @@
         <v>144</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>143</v>
@@ -1043,7 +1030,7 @@
         <v>156</v>
       </c>
       <c r="B2">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A2, ":"),D$2:D$124)))</f>
+        <f t="shared" ref="B2:B33" si="0">SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A2, ":"),D$2:D$124)))</f>
         <v>1</v>
       </c>
       <c r="C2" s="6">
@@ -1060,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1068,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A3, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C3">
@@ -1086,7 +1073,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A4, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C4">
@@ -1107,7 +1094,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A5, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C5">
@@ -1125,23 +1112,23 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>158</v>
-      </c>
-      <c r="B6">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A6, ":"),D$2:D$124)))</f>
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>159</v>
       </c>
       <c r="E6" t="s">
         <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1152,7 +1139,7 @@
         <v>146</v>
       </c>
       <c r="B7">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A7, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C7">
@@ -1165,7 +1152,7 @@
         <v>69</v>
       </c>
       <c r="F7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -1176,7 +1163,7 @@
         <v>57</v>
       </c>
       <c r="B8">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A8, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C8">
@@ -1189,7 +1176,7 @@
         <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1200,7 +1187,7 @@
         <v>58</v>
       </c>
       <c r="B9">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A9, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C9">
@@ -1212,20 +1199,17 @@
       <c r="E9" t="s">
         <v>69</v>
       </c>
-      <c r="F9" t="s">
-        <v>160</v>
-      </c>
       <c r="G9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B10">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A10, ":"),D$2:D$124)))</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1239,17 +1223,17 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
         <v>162</v>
-      </c>
-      <c r="B11">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A11, ":"),D$2:D$124)))</f>
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>163</v>
       </c>
       <c r="E11" t="s">
         <v>69</v>
@@ -1263,7 +1247,7 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A12, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C12">
@@ -1281,7 +1265,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A13, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C13">
@@ -1302,7 +1286,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A14, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C14">
@@ -1323,7 +1307,7 @@
         <v>61</v>
       </c>
       <c r="B15">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A15, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C15">
@@ -1336,7 +1320,7 @@
         <v>69</v>
       </c>
       <c r="F15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G15">
         <v>0</v>
@@ -1347,7 +1331,7 @@
         <v>151</v>
       </c>
       <c r="B16">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A16, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C16">
@@ -1360,7 +1344,7 @@
         <v>72</v>
       </c>
       <c r="F16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1371,7 +1355,7 @@
         <v>59</v>
       </c>
       <c r="B17">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A17, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C17">
@@ -1392,7 +1376,7 @@
         <v>60</v>
       </c>
       <c r="B18">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A18, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C18">
@@ -1409,11 +1393,11 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B19">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A19, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C19">
@@ -1427,11 +1411,11 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B20">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A20, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C20">
@@ -1448,11 +1432,11 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B21">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A21, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C21">
@@ -1473,7 +1457,7 @@
         <v>62</v>
       </c>
       <c r="B22">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A22, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C22">
@@ -1486,7 +1470,7 @@
         <v>69</v>
       </c>
       <c r="F22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1497,7 +1481,7 @@
         <v>6</v>
       </c>
       <c r="B23">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A23, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C23">
@@ -1515,7 +1499,7 @@
         <v>17</v>
       </c>
       <c r="B24">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A24, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C24">
@@ -1536,7 +1520,7 @@
         <v>18</v>
       </c>
       <c r="B25">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A25, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C25">
@@ -1557,7 +1541,7 @@
         <v>7</v>
       </c>
       <c r="B26">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A26, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C26">
@@ -1575,7 +1559,7 @@
         <v>19</v>
       </c>
       <c r="B27">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A27, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C27">
@@ -1596,7 +1580,7 @@
         <v>20</v>
       </c>
       <c r="B28">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A28, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C28">
@@ -1609,7 +1593,7 @@
         <v>72</v>
       </c>
       <c r="F28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1617,23 +1601,23 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29" t="s">
         <v>179</v>
-      </c>
-      <c r="B29">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A29, ":"),D$2:D$124)))</f>
-        <v>0</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>180</v>
       </c>
       <c r="E29" t="s">
         <v>69</v>
       </c>
       <c r="F29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1644,7 +1628,7 @@
         <v>147</v>
       </c>
       <c r="B30">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A30, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C30">
@@ -1657,7 +1641,7 @@
         <v>69</v>
       </c>
       <c r="F30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1668,7 +1652,7 @@
         <v>9</v>
       </c>
       <c r="B31">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A31, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C31">
@@ -1686,7 +1670,7 @@
         <v>21</v>
       </c>
       <c r="B32">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A32, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C32">
@@ -1707,7 +1691,7 @@
         <v>22</v>
       </c>
       <c r="B33">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A33, ":"),D$2:D$124)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C33">
@@ -1724,11 +1708,11 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B34">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A34, ":"),D$2:D$124)))</f>
+        <f t="shared" ref="B34:B65" si="1">SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A34, ":"),D$2:D$124)))</f>
         <v>4</v>
       </c>
       <c r="C34">
@@ -1742,11 +1726,11 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B35">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A35, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C35">
@@ -1763,11 +1747,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B36">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A36, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C36">
@@ -1788,7 +1772,7 @@
         <v>8</v>
       </c>
       <c r="B37">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A37, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C37">
@@ -1806,7 +1790,7 @@
         <v>25</v>
       </c>
       <c r="B38">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A38, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C38">
@@ -1827,7 +1811,7 @@
         <v>26</v>
       </c>
       <c r="B39">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A39, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C39">
@@ -1848,14 +1832,14 @@
         <v>154</v>
       </c>
       <c r="B40">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A40, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C40" s="6">
         <v>0</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>74</v>
@@ -1867,23 +1851,23 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="B41">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A41, ":"),D$2:D$124)))</f>
-        <v>0</v>
-      </c>
-      <c r="C41" s="6">
-        <v>1</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>69</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -1894,7 +1878,7 @@
         <v>27</v>
       </c>
       <c r="B42">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A42, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C42">
@@ -1915,7 +1899,7 @@
         <v>28</v>
       </c>
       <c r="B43">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A43, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C43">
@@ -1936,7 +1920,7 @@
         <v>29</v>
       </c>
       <c r="B44">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A44, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C44">
@@ -1957,7 +1941,7 @@
         <v>30</v>
       </c>
       <c r="B45">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A45, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C45">
@@ -1978,7 +1962,7 @@
         <v>31</v>
       </c>
       <c r="B46">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A46, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C46">
@@ -1999,7 +1983,7 @@
         <v>32</v>
       </c>
       <c r="B47">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A47, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C47">
@@ -2020,7 +2004,7 @@
         <v>33</v>
       </c>
       <c r="B48">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A48, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C48">
@@ -2041,7 +2025,7 @@
         <v>34</v>
       </c>
       <c r="B49">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A49, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C49">
@@ -2062,7 +2046,7 @@
         <v>35</v>
       </c>
       <c r="B50">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A50, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C50">
@@ -2083,7 +2067,7 @@
         <v>115</v>
       </c>
       <c r="B51">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A51, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C51">
@@ -2104,14 +2088,14 @@
         <v>116</v>
       </c>
       <c r="B52">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A52, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C52">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E52" t="s">
         <v>74</v>
@@ -2125,7 +2109,7 @@
         <v>117</v>
       </c>
       <c r="B53">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A53, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C53">
@@ -2138,7 +2122,7 @@
         <v>69</v>
       </c>
       <c r="F53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2146,10 +2130,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B54">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A54, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C54">
@@ -2164,17 +2148,17 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B55">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A55, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E55" t="s">
         <v>72</v>
@@ -2185,23 +2169,23 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B56">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A56, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E56" t="s">
         <v>69</v>
       </c>
       <c r="F56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2212,7 +2196,7 @@
         <v>36</v>
       </c>
       <c r="B57">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A57, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C57">
@@ -2233,7 +2217,7 @@
         <v>37</v>
       </c>
       <c r="B58">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A58, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C58">
@@ -2254,7 +2238,7 @@
         <v>38</v>
       </c>
       <c r="B59">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A59, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C59">
@@ -2275,7 +2259,7 @@
         <v>39</v>
       </c>
       <c r="B60">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A60, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C60">
@@ -2296,7 +2280,7 @@
         <v>40</v>
       </c>
       <c r="B61">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A61, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C61">
@@ -2317,7 +2301,7 @@
         <v>41</v>
       </c>
       <c r="B62">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A62, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C62">
@@ -2338,7 +2322,7 @@
         <v>119</v>
       </c>
       <c r="B63">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A63, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C63">
@@ -2351,7 +2335,7 @@
         <v>69</v>
       </c>
       <c r="F63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2362,7 +2346,7 @@
         <v>42</v>
       </c>
       <c r="B64">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A64, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C64">
@@ -2383,7 +2367,7 @@
         <v>43</v>
       </c>
       <c r="B65">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A65, ":"),D$2:D$124)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C65">
@@ -2404,7 +2388,7 @@
         <v>44</v>
       </c>
       <c r="B66">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A66, ":"),D$2:D$124)))</f>
+        <f t="shared" ref="B66:B97" si="2">SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A66, ":"),D$2:D$124)))</f>
         <v>0</v>
       </c>
       <c r="C66">
@@ -2425,7 +2409,7 @@
         <v>45</v>
       </c>
       <c r="B67">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A67, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C67">
@@ -2443,7 +2427,7 @@
         <v>46</v>
       </c>
       <c r="B68">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A68, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C68">
@@ -2464,7 +2448,7 @@
         <v>47</v>
       </c>
       <c r="B69">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A69, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C69">
@@ -2482,10 +2466,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B70">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A70, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C70">
@@ -2500,14 +2484,14 @@
         <v>48</v>
       </c>
       <c r="B71">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A71, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E71" t="s">
         <v>74</v>
@@ -2521,7 +2505,7 @@
         <v>49</v>
       </c>
       <c r="B72">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A72, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C72">
@@ -2542,7 +2526,7 @@
         <v>50</v>
       </c>
       <c r="B73">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A73, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C73">
@@ -2560,23 +2544,23 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
         <v>171</v>
-      </c>
-      <c r="B74">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A74, ":"),D$2:D$124)))</f>
-        <v>0</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74" t="s">
-        <v>172</v>
       </c>
       <c r="E74" t="s">
         <v>74</v>
       </c>
       <c r="F74" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -2587,7 +2571,7 @@
         <v>51</v>
       </c>
       <c r="B75">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A75, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C75">
@@ -2605,7 +2589,7 @@
         <v>52</v>
       </c>
       <c r="B76">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A76, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C76">
@@ -2626,7 +2610,7 @@
         <v>53</v>
       </c>
       <c r="B77">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A77, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C77">
@@ -2647,7 +2631,7 @@
         <v>54</v>
       </c>
       <c r="B78">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A78, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C78">
@@ -2668,7 +2652,7 @@
         <v>55</v>
       </c>
       <c r="B79">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A79, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C79">
@@ -2689,7 +2673,7 @@
         <v>56</v>
       </c>
       <c r="B80">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A80, ":"),D$2:D$124)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C80">
@@ -2740,7 +2724,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{B41CAD5B-3ED5-49EE-9D16-AE4F85D7209A}">
       <formula1>$A$1:$A$80</formula1>
     </dataValidation>
@@ -2779,7 +2763,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="B8:F8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2885,10 +2869,10 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B13" t="s">
         <v>165</v>
-      </c>
-      <c r="B13" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>